<commit_message>
updated language in supporting info
</commit_message>
<xml_diff>
--- a/Databases/manual_QC.xlsx
+++ b/Databases/manual_QC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdp2019/Desktop/PGD-preop-metabolomics/Databases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D080411-D987-CA4B-BBB3-7EAA4C2465D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864D5E33-D904-9344-9E35-D622A003CA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5060,9 +5060,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA9933B-54E3-1D43-BD07-5F8E6DDF0D45}">
   <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>